<commit_message>
Added many changes in framework
</commit_message>
<xml_diff>
--- a/Data/TestCases.xlsx
+++ b/Data/TestCases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>TCID</t>
   </si>
@@ -81,44 +81,75 @@
     <t>M2</t>
   </si>
   <si>
+    <t>Scripts.Test1</t>
+  </si>
+  <si>
+    <t>Scripts.Test2</t>
+  </si>
+  <si>
+    <t>Scripts.Test3</t>
+  </si>
+  <si>
+    <t>TC004</t>
+  </si>
+  <si>
     <t>chrome</t>
   </si>
   <si>
+    <t>TestCaseD3</t>
+  </si>
+  <si>
+    <t>TC_Verify_EnteredMessage_chrome</t>
+  </si>
+  <si>
+    <t>Scripts.Index.EnterMessage</t>
+  </si>
+  <si>
+    <t>TC005</t>
+  </si>
+  <si>
+    <t>Scripts.Index.VerifyEnteredMessage</t>
+  </si>
+  <si>
+    <t>TC_Verify_VerifyMessage_firefox</t>
+  </si>
+  <si>
     <t>firefox</t>
   </si>
   <si>
-    <t>edge</t>
-  </si>
-  <si>
-    <t>Scripts.Test1</t>
-  </si>
-  <si>
-    <t>Scripts.Test2</t>
-  </si>
-  <si>
-    <t>Scripts.Test3</t>
-  </si>
-  <si>
-    <t>TC004</t>
-  </si>
-  <si>
-    <t>TC_Verify_EnteredMessage</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>Scripts.VerifyMessage</t>
+    <t>Scripts.ListBox.AddAll</t>
+  </si>
+  <si>
+    <t>TC006</t>
+  </si>
+  <si>
+    <t>TC_Verify_ClickAll</t>
+  </si>
+  <si>
+    <t>ListBox</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Lorem ipsum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,14 +175,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -427,51 +491,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:XFC196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10 16383:16383" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="XFC1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10 16383:16383" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -485,25 +552,28 @@
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
         <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
         <v>16</v>
       </c>
       <c r="I2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J2" s="1">
         <v>123456</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="XFC2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10 16383:16383" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -517,24 +587,26 @@
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
         <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
       <c r="J3">
         <v>3345</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10 16383:16383" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -543,47 +615,831 @@
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
         <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
       <c r="J4">
         <v>567</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10 16383:16383" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
         <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:10 16383:16383" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>28</v>
       </c>
-      <c r="E5" t="s">
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
         <v>29</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" t="s">
         <v>14</v>
       </c>
-      <c r="G5" t="s">
-        <v>20</v>
-      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10 16383:16383" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:10 16383:16383" x14ac:dyDescent="0.25">
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:10 16383:16383" x14ac:dyDescent="0.25">
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:10 16383:16383" x14ac:dyDescent="0.25">
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:10 16383:16383" x14ac:dyDescent="0.25">
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:10 16383:16383" x14ac:dyDescent="0.25">
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:10 16383:16383" x14ac:dyDescent="0.25">
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:10 16383:16383" x14ac:dyDescent="0.25">
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:10 16383:16383" x14ac:dyDescent="0.25">
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:10 16383:16383" x14ac:dyDescent="0.25">
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+    </row>
+    <row r="41" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+    </row>
+    <row r="44" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+    </row>
+    <row r="46" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+    </row>
+    <row r="47" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+    </row>
+    <row r="48" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+    </row>
+    <row r="49" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+    </row>
+    <row r="50" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+    </row>
+    <row r="51" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+    </row>
+    <row r="52" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+    </row>
+    <row r="53" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+    </row>
+    <row r="54" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+    </row>
+    <row r="55" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+    </row>
+    <row r="56" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+    </row>
+    <row r="57" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+    </row>
+    <row r="58" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+    </row>
+    <row r="59" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+    </row>
+    <row r="60" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+    </row>
+    <row r="61" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+    </row>
+    <row r="62" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+    </row>
+    <row r="63" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+    </row>
+    <row r="64" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+    </row>
+    <row r="65" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+    </row>
+    <row r="66" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+    </row>
+    <row r="67" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+    </row>
+    <row r="68" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+    </row>
+    <row r="69" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+    </row>
+    <row r="70" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+    </row>
+    <row r="71" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+    </row>
+    <row r="72" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+    </row>
+    <row r="73" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+    </row>
+    <row r="74" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+    </row>
+    <row r="75" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H75" s="2"/>
+      <c r="I75" s="2"/>
+    </row>
+    <row r="76" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+    </row>
+    <row r="77" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+    </row>
+    <row r="78" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+    </row>
+    <row r="79" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H79" s="2"/>
+      <c r="I79" s="2"/>
+    </row>
+    <row r="80" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+    </row>
+    <row r="81" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
+    </row>
+    <row r="82" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
+    </row>
+    <row r="83" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
+    </row>
+    <row r="84" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H84" s="2"/>
+      <c r="I84" s="2"/>
+    </row>
+    <row r="85" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
+    </row>
+    <row r="86" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
+    </row>
+    <row r="87" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+    </row>
+    <row r="88" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H88" s="2"/>
+      <c r="I88" s="2"/>
+    </row>
+    <row r="89" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H89" s="2"/>
+      <c r="I89" s="2"/>
+    </row>
+    <row r="90" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H90" s="2"/>
+      <c r="I90" s="2"/>
+    </row>
+    <row r="91" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H91" s="2"/>
+      <c r="I91" s="2"/>
+    </row>
+    <row r="92" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+    </row>
+    <row r="93" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H93" s="2"/>
+      <c r="I93" s="2"/>
+    </row>
+    <row r="94" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H94" s="2"/>
+      <c r="I94" s="2"/>
+    </row>
+    <row r="95" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H95" s="2"/>
+      <c r="I95" s="2"/>
+    </row>
+    <row r="96" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H96" s="2"/>
+      <c r="I96" s="2"/>
+    </row>
+    <row r="97" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H97" s="2"/>
+      <c r="I97" s="2"/>
+    </row>
+    <row r="98" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H98" s="2"/>
+      <c r="I98" s="2"/>
+    </row>
+    <row r="99" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H99" s="2"/>
+      <c r="I99" s="2"/>
+    </row>
+    <row r="100" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H100" s="2"/>
+      <c r="I100" s="2"/>
+    </row>
+    <row r="101" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
+    </row>
+    <row r="102" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H102" s="2"/>
+      <c r="I102" s="2"/>
+    </row>
+    <row r="103" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H103" s="2"/>
+      <c r="I103" s="2"/>
+    </row>
+    <row r="104" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H104" s="2"/>
+      <c r="I104" s="2"/>
+    </row>
+    <row r="105" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H105" s="2"/>
+      <c r="I105" s="2"/>
+    </row>
+    <row r="106" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H106" s="2"/>
+      <c r="I106" s="2"/>
+    </row>
+    <row r="107" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H107" s="2"/>
+      <c r="I107" s="2"/>
+    </row>
+    <row r="108" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H108" s="2"/>
+      <c r="I108" s="2"/>
+    </row>
+    <row r="109" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H109" s="2"/>
+      <c r="I109" s="2"/>
+    </row>
+    <row r="110" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H110" s="2"/>
+      <c r="I110" s="2"/>
+    </row>
+    <row r="111" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H111" s="2"/>
+      <c r="I111" s="2"/>
+    </row>
+    <row r="112" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H112" s="2"/>
+      <c r="I112" s="2"/>
+    </row>
+    <row r="113" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H113" s="2"/>
+      <c r="I113" s="2"/>
+    </row>
+    <row r="114" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H114" s="2"/>
+      <c r="I114" s="2"/>
+    </row>
+    <row r="115" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H115" s="2"/>
+      <c r="I115" s="2"/>
+    </row>
+    <row r="116" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H116" s="2"/>
+      <c r="I116" s="2"/>
+    </row>
+    <row r="117" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H117" s="2"/>
+      <c r="I117" s="2"/>
+    </row>
+    <row r="118" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H118" s="2"/>
+      <c r="I118" s="2"/>
+    </row>
+    <row r="119" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H119" s="2"/>
+      <c r="I119" s="2"/>
+    </row>
+    <row r="120" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H120" s="2"/>
+      <c r="I120" s="2"/>
+    </row>
+    <row r="121" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H121" s="2"/>
+      <c r="I121" s="2"/>
+    </row>
+    <row r="122" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H122" s="2"/>
+      <c r="I122" s="2"/>
+    </row>
+    <row r="123" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H123" s="2"/>
+      <c r="I123" s="2"/>
+    </row>
+    <row r="124" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H124" s="2"/>
+      <c r="I124" s="2"/>
+    </row>
+    <row r="125" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H125" s="2"/>
+      <c r="I125" s="2"/>
+    </row>
+    <row r="126" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H126" s="2"/>
+      <c r="I126" s="2"/>
+    </row>
+    <row r="127" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H127" s="2"/>
+      <c r="I127" s="2"/>
+    </row>
+    <row r="128" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H128" s="2"/>
+      <c r="I128" s="2"/>
+    </row>
+    <row r="129" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H129" s="2"/>
+      <c r="I129" s="2"/>
+    </row>
+    <row r="130" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H130" s="2"/>
+      <c r="I130" s="2"/>
+    </row>
+    <row r="131" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H131" s="2"/>
+      <c r="I131" s="2"/>
+    </row>
+    <row r="132" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H132" s="2"/>
+      <c r="I132" s="2"/>
+    </row>
+    <row r="133" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H133" s="2"/>
+      <c r="I133" s="2"/>
+    </row>
+    <row r="134" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H134" s="2"/>
+      <c r="I134" s="2"/>
+    </row>
+    <row r="135" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H135" s="2"/>
+      <c r="I135" s="2"/>
+    </row>
+    <row r="136" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H136" s="2"/>
+      <c r="I136" s="2"/>
+    </row>
+    <row r="137" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H137" s="2"/>
+      <c r="I137" s="2"/>
+    </row>
+    <row r="138" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H138" s="2"/>
+      <c r="I138" s="2"/>
+    </row>
+    <row r="139" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H139" s="2"/>
+      <c r="I139" s="2"/>
+    </row>
+    <row r="140" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H140" s="2"/>
+      <c r="I140" s="2"/>
+    </row>
+    <row r="141" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H141" s="2"/>
+      <c r="I141" s="2"/>
+    </row>
+    <row r="142" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H142" s="2"/>
+      <c r="I142" s="2"/>
+    </row>
+    <row r="143" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H143" s="2"/>
+      <c r="I143" s="2"/>
+    </row>
+    <row r="144" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H144" s="2"/>
+      <c r="I144" s="2"/>
+    </row>
+    <row r="145" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H145" s="2"/>
+      <c r="I145" s="2"/>
+    </row>
+    <row r="146" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H146" s="2"/>
+      <c r="I146" s="2"/>
+    </row>
+    <row r="147" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H147" s="2"/>
+      <c r="I147" s="2"/>
+    </row>
+    <row r="148" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H148" s="2"/>
+      <c r="I148" s="2"/>
+    </row>
+    <row r="149" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H149" s="2"/>
+      <c r="I149" s="2"/>
+    </row>
+    <row r="150" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H150" s="2"/>
+      <c r="I150" s="2"/>
+    </row>
+    <row r="151" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H151" s="2"/>
+      <c r="I151" s="2"/>
+    </row>
+    <row r="152" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H152" s="2"/>
+      <c r="I152" s="2"/>
+    </row>
+    <row r="153" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H153" s="2"/>
+      <c r="I153" s="2"/>
+    </row>
+    <row r="154" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H154" s="2"/>
+      <c r="I154" s="2"/>
+    </row>
+    <row r="155" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="I155" s="2"/>
+    </row>
+    <row r="156" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="I156" s="2"/>
+    </row>
+    <row r="157" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="I157" s="2"/>
+    </row>
+    <row r="158" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="I158" s="2"/>
+    </row>
+    <row r="159" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="I159" s="2"/>
+    </row>
+    <row r="160" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="I160" s="2"/>
+    </row>
+    <row r="161" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I161" s="2"/>
+    </row>
+    <row r="162" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I162" s="2"/>
+    </row>
+    <row r="163" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I163" s="2"/>
+    </row>
+    <row r="164" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I164" s="2"/>
+    </row>
+    <row r="165" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I165" s="2"/>
+    </row>
+    <row r="166" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I166" s="2"/>
+    </row>
+    <row r="167" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I167" s="2"/>
+    </row>
+    <row r="168" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I168" s="2"/>
+    </row>
+    <row r="169" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I169" s="2"/>
+    </row>
+    <row r="170" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I170" s="2"/>
+    </row>
+    <row r="171" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I171" s="2"/>
+    </row>
+    <row r="172" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I172" s="2"/>
+    </row>
+    <row r="173" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I173" s="2"/>
+    </row>
+    <row r="174" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I174" s="2"/>
+    </row>
+    <row r="175" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I175" s="2"/>
+    </row>
+    <row r="176" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I176" s="2"/>
+    </row>
+    <row r="177" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I177" s="2"/>
+    </row>
+    <row r="178" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I178" s="2"/>
+    </row>
+    <row r="179" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I179" s="2"/>
+    </row>
+    <row r="180" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I180" s="2"/>
+    </row>
+    <row r="181" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I181" s="2"/>
+    </row>
+    <row r="182" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I182" s="2"/>
+    </row>
+    <row r="183" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I183" s="2"/>
+    </row>
+    <row r="184" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I184" s="2"/>
+    </row>
+    <row r="185" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I185" s="2"/>
+    </row>
+    <row r="186" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I186" s="2"/>
+    </row>
+    <row r="187" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I187" s="2"/>
+    </row>
+    <row r="188" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I188" s="2"/>
+    </row>
+    <row r="189" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I189" s="2"/>
+    </row>
+    <row r="190" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I190" s="2"/>
+    </row>
+    <row r="191" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I191" s="2"/>
+    </row>
+    <row r="192" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I192" s="2"/>
+    </row>
+    <row r="193" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I193" s="2"/>
+    </row>
+    <row r="194" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I194" s="2"/>
+    </row>
+    <row r="195" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I195" s="2"/>
+    </row>
+    <row r="196" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I196" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H5">
+  <conditionalFormatting sqref="B7:B1048576 B2:B4">
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I196 H2:H154">
       <formula1>$W$2:$W$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6 C2:C6">
+      <formula1>$XFC$1:$XFC$2</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>